<commit_message>
Made changes to IRP package and where files are referenced in code.
</commit_message>
<xml_diff>
--- a/irp-webapp/src/main/resources/irp-package/Training Test 10th Grade Math Items (with sample Student Responses).xlsx
+++ b/irp-webapp/src/main/resources/irp-package/Training Test 10th Grade Math Items (with sample Student Responses).xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="29020" windowHeight="27040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -186,15 +186,6 @@
     <t>Training Test Item</t>
   </si>
   <si>
-    <t>Student 1 Response</t>
-  </si>
-  <si>
-    <t>Student 2 Response</t>
-  </si>
-  <si>
-    <t>Student 3 Response</t>
-  </si>
-  <si>
     <t>any text</t>
   </si>
   <si>
@@ -277,6 +268,15 @@
   </si>
   <si>
     <t>Training Test Items (corresponding to Column J above)</t>
+  </si>
+  <si>
+    <t>Student SSID 8598 Response</t>
+  </si>
+  <si>
+    <t>Student SSID 8599 Response</t>
+  </si>
+  <si>
+    <t>Student SSID 8600 Response</t>
   </si>
 </sst>
 </file>
@@ -1133,7 +1133,7 @@
   <dimension ref="A1:AE20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1142,7 +1142,9 @@
     <col min="2" max="2" width="13.1640625" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" customWidth="1"/>
     <col min="10" max="10" width="17.33203125" style="8" customWidth="1"/>
-    <col min="11" max="13" width="17.33203125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="25.1640625" style="11" customWidth="1"/>
+    <col min="12" max="12" width="23.6640625" style="11" customWidth="1"/>
+    <col min="13" max="13" width="22.83203125" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
@@ -1182,7 +1184,7 @@
       <c r="AD1" s="4"/>
       <c r="AE1" s="4"/>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:31" ht="28">
       <c r="A2" s="5" t="s">
         <v>32</v>
       </c>
@@ -1214,13 +1216,13 @@
         <v>54</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="O2" s="7" t="s">
         <v>41</v>
@@ -1303,13 +1305,13 @@
         <v>2</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="O3">
         <v>174</v>
@@ -1392,13 +1394,13 @@
         <v>3</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="O4">
         <v>666</v>
@@ -1570,13 +1572,13 @@
         <v>8</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="O6">
         <v>766</v>
@@ -1659,13 +1661,13 @@
         <v>1</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O7">
         <v>769</v>
@@ -1716,7 +1718,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="30">
+    <row r="8" spans="1:31">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1748,13 +1750,13 @@
         <v>6</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="O8">
         <v>1059</v>
@@ -1834,16 +1836,16 @@
         <v>1387</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="O9">
         <v>1387</v>
@@ -1923,16 +1925,16 @@
         <v>1448</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="O10">
         <v>1448</v>
@@ -2015,13 +2017,13 @@
         <v>7</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="O11">
         <v>1672</v>
@@ -2104,13 +2106,13 @@
         <v>5</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="O12">
         <v>1676</v>
@@ -2190,16 +2192,16 @@
         <v>1688</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="O13">
         <v>1688</v>
@@ -2252,7 +2254,7 @@
     </row>
     <row r="19" spans="1:10" ht="26" thickBot="1">
       <c r="A19" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>

</xml_diff>